<commit_message>
AAI finished, started tests-writing
</commit_message>
<xml_diff>
--- a/stimuls.xlsx
+++ b/stimuls.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>index</t>
   </si>
@@ -39,16 +39,31 @@
     <t>QRS_index</t>
   </si>
   <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>undersensing</t>
+  </si>
+  <si>
+    <t>exactlyUndersensing</t>
+  </si>
+  <si>
+    <t>oversensing</t>
+  </si>
+  <si>
+    <t>noAnswer</t>
+  </si>
+  <si>
+    <t>unrelized</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
     <t>AU</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>AN</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
 </sst>
 </file>
@@ -400,13 +415,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,356 +434,675 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>869</v>
+        <v>3196</v>
       </c>
       <c r="D2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>914</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>1619</v>
+        <v>3863</v>
       </c>
       <c r="D3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>876</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>2369</v>
+        <v>4531</v>
       </c>
       <c r="D4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>876</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>3119</v>
+        <v>5198</v>
       </c>
       <c r="D5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>660</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>3869</v>
+        <v>5866</v>
       </c>
       <c r="D6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>916</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>4619</v>
+        <v>6533</v>
       </c>
       <c r="D7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>916</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>5369</v>
+        <v>7201</v>
       </c>
       <c r="D8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>876</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>6119</v>
+        <v>7868</v>
       </c>
       <c r="D9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>876</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>6869</v>
+        <v>8536</v>
       </c>
       <c r="D10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>546</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>7619</v>
+        <v>9211</v>
       </c>
       <c r="D11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>1116</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>8369</v>
+        <v>9886</v>
       </c>
       <c r="D12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>1116</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>9119</v>
+        <v>10561</v>
       </c>
       <c r="D13">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>916</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>9869</v>
+        <v>11236</v>
       </c>
       <c r="D14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>916</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>10619</v>
+        <v>11912</v>
       </c>
       <c r="D15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>874</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>11370</v>
+        <v>12587</v>
       </c>
       <c r="D16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>874</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C17">
-        <v>12120</v>
+        <v>13262</v>
       </c>
       <c r="D17">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>680</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C18">
-        <v>12870</v>
+        <v>13935</v>
       </c>
       <c r="D18">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>936</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>13620</v>
+        <v>14612</v>
       </c>
       <c r="D19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>936</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>14368</v>
+        <v>15285</v>
       </c>
       <c r="D20">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>585</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C21">
-        <v>15118</v>
+        <v>15960</v>
       </c>
       <c r="D21">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>755</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C22">
-        <v>15868</v>
+        <v>16643</v>
       </c>
       <c r="D22">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>691</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>16618</v>
+        <v>17325</v>
       </c>
       <c r="D23">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>934</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>17368</v>
+        <v>18008</v>
       </c>
       <c r="D24">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>27</v>
+      </c>
+      <c r="E24">
+        <v>934</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>18118</v>
+        <v>18690</v>
       </c>
       <c r="D25">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26">
-        <v>18868</v>
-      </c>
-      <c r="D26">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E25">
+        <v>680</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>